<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@5eec434a8f168485e7d8f30478db3dc96ed593f2 🚀
</commit_message>
<xml_diff>
--- a/castor.xlsx
+++ b/castor.xlsx
@@ -332,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -524,6 +524,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1496,7 +1499,11 @@
       <c r="J6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="59"/>
+      <c r="L6" s="59" t="inlineStr">
+        <is>
+          <t>1/2 journée</t>
+        </is>
+      </c>
       <c r="M6" s="59"/>
       <c r="N6" s="4"/>
       <c r="O6" s="62"/>
@@ -1568,7 +1575,11 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="7"/>
-      <c r="O9" s="63"/>
+      <c r="O9" s="63" t="inlineStr">
+        <is>
+          <t>Formation Petit et Méso-Carnivores et Castor</t>
+        </is>
+      </c>
       <c r="P9" s="64"/>
       <c r="Q9" s="65"/>
       <c r="R9" s="31"/>
@@ -1610,9 +1621,24 @@
       <c r="H11" s="78"/>
       <c r="I11" s="5"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="47"/>
+      <c r="K11" s="70" t="inlineStr">
+        <is>
+          <t>Animation
+Base de données
+Formation</t>
+        </is>
+      </c>
+      <c r="L11" s="70" t="inlineStr">
+        <is>
+          <t>Coordination
+Remontée des données au national</t>
+        </is>
+      </c>
+      <c r="M11" s="47" t="inlineStr">
+        <is>
+          <t>Prospections</t>
+        </is>
+      </c>
       <c r="N11" s="46"/>
       <c r="O11" s="63"/>
       <c r="P11" s="64"/>
@@ -1741,11 +1767,22 @@
       <c r="H16" s="46"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="47"/>
+      <c r="K16" s="47" t="inlineStr">
+        <is>
+          <t>Recherche d'indices de présence (bois coupé, écorçage, hutte…) en prospection sur l'eau et à pied en berge</t>
+        </is>
+      </c>
       <c r="L16" s="45"/>
       <c r="M16" s="45"/>
       <c r="N16" s="46"/>
-      <c r="O16" s="47"/>
+      <c r="O16" s="47" t="inlineStr">
+        <is>
+          <t>kayak
+gilet de sauvetage
+jumelles
+appareil photo</t>
+        </is>
+      </c>
       <c r="P16" s="45"/>
       <c r="Q16" s="46"/>
       <c r="R16" s="5"/>
@@ -2105,7 +2142,11 @@
       <c r="I33" s="5"/>
       <c r="J33" s="4"/>
       <c r="K33" s="8"/>
-      <c r="L33" s="45"/>
+      <c r="L33" s="45" t="inlineStr">
+        <is>
+          <t>Remplissage des fiches terrains et transmission à l'animateur régional</t>
+        </is>
+      </c>
       <c r="M33" s="45"/>
       <c r="N33" s="46"/>
       <c r="O33" s="47" t="inlineStr">
@@ -2303,7 +2344,11 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="37"/>
+      <c r="B43" s="37" t="inlineStr">
+        <is>
+          <t>Prospections hivernales avant la reprise de la végétation</t>
+        </is>
+      </c>
       <c r="C43" s="38"/>
       <c r="D43" s="38"/>
       <c r="E43" s="38"/>
@@ -2399,7 +2444,9 @@
         <v>18</v>
       </c>
       <c r="K47" s="2"/>
-      <c r="L47" s="43"/>
+      <c r="L47" s="81" t="str">
+        <f>=HYPERLINK("https://ged.ofb.fr/share/page/site/dridf-rseau-partenarial-castor/dashboard", "Site Alfresco du Réseau Castor IdF")</f>
+      </c>
       <c r="M47" s="43"/>
       <c r="N47" s="43"/>
       <c r="O47" s="43"/>
@@ -2421,7 +2468,9 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="L48" s="69"/>
+      <c r="L48" s="83" t="str">
+        <f>=HYPERLINK("https://ged.ofb.fr/share/s/giB4EPFIRPmsQZiGFeYY0A", "Protocole")</f>
+      </c>
       <c r="M48" s="69"/>
       <c r="N48" s="69"/>
       <c r="O48" s="69"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@40fde0e617cadfbdbe3027b90dcd3e6b35f36185 🚀
</commit_message>
<xml_diff>
--- a/castor.xlsx
+++ b/castor.xlsx
@@ -1777,10 +1777,11 @@
       <c r="N16" s="46"/>
       <c r="O16" s="47" t="inlineStr">
         <is>
-          <t>kayak
-gilet de sauvetage
-jumelles
-appareil photo</t>
+          <t>- embarquation (ex. kayak)
+- gilet de sauvetage
+- jumelles
+- appareil photo
+- GPS</t>
         </is>
       </c>
       <c r="P16" s="45"/>
@@ -2144,7 +2145,9 @@
       <c r="K33" s="8"/>
       <c r="L33" s="45" t="inlineStr">
         <is>
-          <t>Remplissage des fiches terrains et transmission à l'animateur régional</t>
+          <t xml:space="preserve">Remplissage des fiches terrains
+Bancarisation régionale
+Transmission au national </t>
         </is>
       </c>
       <c r="M33" s="45"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@0899c10984fc0dc0cf02e077e431d8d5017fdaed 🚀
</commit_message>
<xml_diff>
--- a/castor.xlsx
+++ b/castor.xlsx
@@ -1501,7 +1501,7 @@
       </c>
       <c r="L6" s="59" t="inlineStr">
         <is>
-          <t>1/2 journée</t>
+          <t>environ 1/2 journée par prospection</t>
         </is>
       </c>
       <c r="M6" s="59"/>
@@ -1538,8 +1538,7 @@
       </c>
       <c r="C8" s="57" t="inlineStr">
         <is>
-          <t>Le Castor d'Europe est un mammifère semi-aquatique, et l'un des plus grand rongeur de la planète.
-Cette espèce protégée est une "ingénieure des écosystèmes" au travers des différents aménagements qu'elle réalise dans les cours d'eau.</t>
+          <t>Quasi disparu en Europe au début du 20ème siècle, la prise de mesure de protection du Castor d’Europe à partir de 1909 puis son classement en « espèce protégée » en 1968 a permis leur reconquête du territoire. L’ Ile-de-France est l’un des fronts de colonisation, induisant un suivi annuel et précis permettant de détecter la présence, suivre la distribution de l’espèce et la protéger en conséquence (notamment via l’interdiction de piégeage).</t>
         </is>
       </c>
       <c r="D8" s="57"/>
@@ -1577,7 +1576,8 @@
       <c r="N9" s="7"/>
       <c r="O9" s="63" t="inlineStr">
         <is>
-          <t>Formation Petit et Méso-Carnivores et Castor</t>
+          <t>Formation Petit et Méso-Carnivores et Castor
+(Formation dommage)</t>
         </is>
       </c>
       <c r="P9" s="64"/>
@@ -1636,7 +1636,8 @@
       </c>
       <c r="M11" s="47" t="inlineStr">
         <is>
-          <t>Prospections</t>
+          <t>Prospections
+(Constats de dommage)</t>
         </is>
       </c>
       <c r="N11" s="46"/>
@@ -1689,6 +1690,8 @@
 Paul Hurel
 Suivi scientifique:
 Yoann Bressan
+Couriel du réseau:
+reseau.castor@ofb.gouv.fr
 Animation régionale:
 Cédric Mondy</t>
         </is>
@@ -2025,7 +2028,7 @@
       <c r="F28" s="39"/>
       <c r="G28" s="47" t="inlineStr">
         <is>
-          <t>ENS
+          <t>Conseils départementaux (ENS)
 Syndicats de rivière</t>
         </is>
       </c>
@@ -2145,9 +2148,9 @@
       <c r="K33" s="8"/>
       <c r="L33" s="45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Remplissage des fiches terrains
+          <t>Remplissage des fiches terrains
 Bancarisation régionale
-Transmission au national </t>
+Transmission au national qui effectue une validation et consolidation nationale des données</t>
         </is>
       </c>
       <c r="M33" s="45"/>
@@ -2349,7 +2352,7 @@
       <c r="A43" s="5"/>
       <c r="B43" s="37" t="inlineStr">
         <is>
-          <t>Prospections hivernales avant la reprise de la végétation</t>
+          <t>Prospections préférentiellement hivernales avant la reprise de la végétation</t>
         </is>
       </c>
       <c r="C43" s="38"/>
@@ -2497,7 +2500,9 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
-      <c r="L49" s="69"/>
+      <c r="L49" s="83" t="str">
+        <f>=HYPERLINK("\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Castor\04_ArretesPiegeage", "Arrêtés piégeage (Serveur DR)")</f>
+      </c>
       <c r="M49" s="69"/>
       <c r="N49" s="69"/>
       <c r="O49" s="69"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@826a49c86918253a79612831db07b2b573d6b314 🚀
</commit_message>
<xml_diff>
--- a/castor.xlsx
+++ b/castor.xlsx
@@ -1686,9 +1686,7 @@
       <c r="F13" s="46"/>
       <c r="G13" s="47" t="inlineStr">
         <is>
-          <t>Courriel du réseau:
-reseau.castor@ofb.gouv.fr
-Animation nationale:
+          <t>Animation nationale:
 Paul HUREL
 Suivi scientifique:
 Yoann BRESSAN
@@ -1698,7 +1696,9 @@
 PPC: 
 77: Anne-Gaëlle BLANC
 78-95: Amandine EVRARD
-91: Cyril KLEINPRINZ</t>
+91: Cyril KLEINPRINZ
+Courriel du réseau:
+reseau.castor@ofb.gouv.fr</t>
         </is>
       </c>
       <c r="H13" s="46"/>

</xml_diff>